<commit_message>
addition by the customer: links to the elements
</commit_message>
<xml_diff>
--- a/БАЗА школ на САЙТ исправленное.xlsx
+++ b/БАЗА школ на САЙТ исправленное.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vipda\Desktop\Создание сайта\yandex_map_with_filtermenu-main\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73C2F12-33F0-455B-BC57-4D2DF3E0C241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Информация" sheetId="1" r:id="rId1"/>
@@ -13,7 +19,7 @@
   <definedNames>
     <definedName name="Z_92EB5070_C363_490E_8829_DE1B7D957098_.wvu.FilterData" localSheetId="0" hidden="1">Информация!$A$1:$AT$74</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="Фильтр 1" guid="{92EB5070-C363-490E-8829-DE1B7D957098}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="269">
   <si>
     <t>Название школы</t>
   </si>
@@ -834,12 +840,18 @@
   <si>
     <t>Кол-во ячеек не из 1 или 0</t>
   </si>
+  <si>
+    <t>Ссылка</t>
+  </si>
+  <si>
+    <t>https://mylomonosov.info/school/detail/gosudarstvennoe_byudzhetnoe_obshcheobrazovatelnoe_uchrezhdenie_goroda_moskvy_-shkola_-_1557_imeni_pe/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -864,6 +876,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -898,10 +917,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -942,8 +962,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1164,17 +1189,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:BB997"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AT2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L98" sqref="L98"/>
+      <selection pane="bottomRight" activeCell="BB4" sqref="BB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1374,6 +1399,9 @@
       <c r="AZ1" s="4" t="s">
         <v>264</v>
       </c>
+      <c r="BA1" s="14" t="s">
+        <v>267</v>
+      </c>
       <c r="BB1" s="4" t="s">
         <v>266</v>
       </c>
@@ -1540,6 +1568,9 @@
       <c r="AZ2">
         <f>SUM(C2:M2)</f>
         <v>10</v>
+      </c>
+      <c r="BA2" s="15" t="s">
+        <v>268</v>
       </c>
       <c r="BB2">
         <f>4708 - COUNTIF(C2:AT108,"1") - COUNTIF(C2:AT108,"0")</f>
@@ -62495,7 +62526,7 @@
   <customSheetViews>
     <customSheetView guid="{92EB5070-C363-490E-8829-DE1B7D957098}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AZ74"/>
+      <autoFilter ref="A1:AZ74" xr:uid="{BB100B30-6096-4C06-B53C-3BD2803EED44}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="AV2:AZ108">
@@ -62511,13 +62542,16 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="BA2" r:id="rId1" xr:uid="{63FFC23F-E720-4F4A-A4CE-1F0107D3E18F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>